<commit_message>
Web view and data fixes
</commit_message>
<xml_diff>
--- a/Bracket Generator/Bracket.xlsx
+++ b/Bracket Generator/Bracket.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ben/Dropbox/Developer/March-Madness-Analyzer/Bracket Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E2FB13-22DC-1744-B3DC-1551E9554C34}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,8 +28,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Helvetica Neue"/>
@@ -36,6 +37,11 @@
     <font>
       <sz val="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,16 +108,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -123,6 +129,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -447,11 +456,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57:D64"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,7 +468,7 @@
     <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -484,14 +493,26 @@
       <c r="I1" s="8">
         <v>1</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J1" s="10">
+        <v>1</v>
+      </c>
+      <c r="K1" s="10">
+        <v>1</v>
+      </c>
+      <c r="L1" s="10">
+        <v>1</v>
+      </c>
+      <c r="M1" s="10">
+        <v>1</v>
+      </c>
+      <c r="N1" s="12">
+        <v>1</v>
+      </c>
+      <c r="O1" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>16</v>
       </c>
@@ -511,13 +532,11 @@
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>8</v>
       </c>
-      <c r="B3" s="9">
-        <v>8</v>
-      </c>
+      <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -526,14 +545,16 @@
       <c r="I3" s="6">
         <v>8</v>
       </c>
-      <c r="J3" s="9"/>
+      <c r="J3" s="9">
+        <v>9</v>
+      </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>9</v>
       </c>
@@ -553,15 +574,13 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>5</v>
       </c>
-      <c r="B5" s="9">
-        <v>5</v>
-      </c>
+      <c r="B5" s="9"/>
       <c r="C5" s="9">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -570,14 +589,18 @@
       <c r="I5" s="6">
         <v>5</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="J5" s="9">
+        <v>5</v>
+      </c>
+      <c r="K5" s="9">
+        <v>5</v>
+      </c>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>12</v>
       </c>
@@ -597,12 +620,12 @@
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" s="9">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -612,14 +635,16 @@
       <c r="I7" s="6">
         <v>4</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="9">
+        <v>13</v>
+      </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>13</v>
       </c>
@@ -639,13 +664,11 @@
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="9">
-        <v>6</v>
-      </c>
+      <c r="B9" s="9"/>
       <c r="C9" s="9">
         <v>3</v>
       </c>
@@ -658,14 +681,20 @@
       <c r="I9" s="6">
         <v>6</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="J9" s="9">
+        <v>6</v>
+      </c>
+      <c r="K9" s="9">
+        <v>3</v>
+      </c>
+      <c r="L9" s="9">
+        <v>3</v>
+      </c>
       <c r="M9" s="9"/>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>11</v>
       </c>
@@ -685,7 +714,7 @@
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -700,14 +729,16 @@
       <c r="I11" s="6">
         <v>3</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="9">
+        <v>3</v>
+      </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>14</v>
       </c>
@@ -727,13 +758,11 @@
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>7</v>
       </c>
-      <c r="B13" s="9">
-        <v>10</v>
-      </c>
+      <c r="B13" s="9"/>
       <c r="C13" s="9">
         <v>2</v>
       </c>
@@ -744,14 +773,18 @@
       <c r="I13" s="6">
         <v>7</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+      <c r="J13" s="9">
+        <v>10</v>
+      </c>
+      <c r="K13" s="9">
+        <v>10</v>
+      </c>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -771,7 +804,7 @@
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -786,14 +819,16 @@
       <c r="I15" s="6">
         <v>2</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="9">
+        <v>2</v>
+      </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -813,7 +848,7 @@
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -821,27 +856,35 @@
         <v>1</v>
       </c>
       <c r="C17" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
       </c>
       <c r="E17" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="I17" s="8">
         <v>1</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="J17" s="10">
+        <v>1</v>
+      </c>
+      <c r="K17" s="10">
+        <v>1</v>
+      </c>
+      <c r="L17" s="10">
+        <v>1</v>
+      </c>
+      <c r="M17" s="10">
+        <v>2</v>
+      </c>
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -861,13 +904,11 @@
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>8</v>
       </c>
-      <c r="B19" s="9">
-        <v>9</v>
-      </c>
+      <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -876,14 +917,16 @@
       <c r="I19" s="6">
         <v>8</v>
       </c>
-      <c r="J19" s="9"/>
+      <c r="J19" s="9">
+        <v>9</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>9</v>
       </c>
@@ -904,7 +947,7 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>5</v>
       </c>
@@ -912,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -921,14 +964,18 @@
       <c r="I21" s="6">
         <v>5</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="J21" s="9">
+        <v>5</v>
+      </c>
+      <c r="K21" s="9">
+        <v>4</v>
+      </c>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>12</v>
       </c>
@@ -948,13 +995,11 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>4</v>
       </c>
-      <c r="B23" s="9">
-        <v>4</v>
-      </c>
+      <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -963,14 +1008,16 @@
       <c r="I23" s="6">
         <v>4</v>
       </c>
-      <c r="J23" s="9"/>
+      <c r="J23" s="9">
+        <v>4</v>
+      </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>13</v>
       </c>
@@ -990,18 +1037,16 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>6</v>
       </c>
-      <c r="B25" s="9">
-        <v>6</v>
-      </c>
+      <c r="B25" s="9"/>
       <c r="C25" s="9">
         <v>3</v>
       </c>
       <c r="D25" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="12"/>
@@ -1009,14 +1054,20 @@
       <c r="I25" s="6">
         <v>6</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
+      <c r="J25" s="9">
+        <v>6</v>
+      </c>
+      <c r="K25" s="9">
+        <v>3</v>
+      </c>
+      <c r="L25" s="9">
+        <v>2</v>
+      </c>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -1036,7 +1087,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>3</v>
       </c>
@@ -1051,14 +1102,16 @@
       <c r="I27" s="6">
         <v>3</v>
       </c>
-      <c r="J27" s="9"/>
+      <c r="J27" s="9">
+        <v>3</v>
+      </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>14</v>
       </c>
@@ -1078,13 +1131,11 @@
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>7</v>
       </c>
-      <c r="B29" s="9">
-        <v>7</v>
-      </c>
+      <c r="B29" s="9"/>
       <c r="C29" s="9">
         <v>2</v>
       </c>
@@ -1095,14 +1146,18 @@
       <c r="I29" s="6">
         <v>7</v>
       </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="J29" s="9">
+        <v>7</v>
+      </c>
+      <c r="K29" s="9">
+        <v>2</v>
+      </c>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
       <c r="O29" s="12"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>10</v>
       </c>
@@ -1122,7 +1177,7 @@
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -1137,14 +1192,16 @@
       <c r="I31" s="6">
         <v>2</v>
       </c>
-      <c r="J31" s="9"/>
+      <c r="J31" s="9">
+        <v>2</v>
+      </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>15</v>
       </c>
@@ -1164,7 +1221,7 @@
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -1187,14 +1244,24 @@
       <c r="I33" s="8">
         <v>1</v>
       </c>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
+      <c r="J33" s="10">
+        <v>1</v>
+      </c>
+      <c r="K33" s="10">
+        <v>8</v>
+      </c>
+      <c r="L33" s="10">
+        <v>8</v>
+      </c>
+      <c r="M33" s="10">
+        <v>8</v>
+      </c>
+      <c r="N33" s="10">
+        <v>8</v>
+      </c>
       <c r="O33" s="12"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>16</v>
       </c>
@@ -1214,13 +1281,11 @@
       <c r="N34" s="9"/>
       <c r="O34" s="12"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>8</v>
       </c>
-      <c r="B35" s="9">
-        <v>8</v>
-      </c>
+      <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -1229,14 +1294,16 @@
       <c r="I35" s="6">
         <v>8</v>
       </c>
-      <c r="J35" s="9"/>
+      <c r="J35" s="9">
+        <v>8</v>
+      </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
       <c r="O35" s="12"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>9</v>
       </c>
@@ -1256,15 +1323,15 @@
       <c r="N36" s="9"/>
       <c r="O36" s="12"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>5</v>
       </c>
       <c r="B37" s="9">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C37" s="9">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -1273,14 +1340,18 @@
       <c r="I37" s="6">
         <v>5</v>
       </c>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
+      <c r="J37" s="9">
+        <v>12</v>
+      </c>
+      <c r="K37" s="9">
+        <v>12</v>
+      </c>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
       <c r="O37" s="12"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>12</v>
       </c>
@@ -1300,13 +1371,11 @@
       <c r="N38" s="9"/>
       <c r="O38" s="12"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>4</v>
       </c>
-      <c r="B39" s="9">
-        <v>4</v>
-      </c>
+      <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -1315,14 +1384,16 @@
       <c r="I39" s="6">
         <v>4</v>
       </c>
-      <c r="J39" s="9"/>
+      <c r="J39" s="9">
+        <v>4</v>
+      </c>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="12"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>13</v>
       </c>
@@ -1342,18 +1413,14 @@
       <c r="N40" s="9"/>
       <c r="O40" s="12"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>6</v>
       </c>
-      <c r="B41" s="9">
-        <v>11</v>
-      </c>
-      <c r="C41" s="9">
-        <v>3</v>
-      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -1361,14 +1428,20 @@
       <c r="I41" s="6">
         <v>6</v>
       </c>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
+      <c r="J41" s="9">
+        <v>6</v>
+      </c>
+      <c r="K41" s="9">
+        <v>6</v>
+      </c>
+      <c r="L41" s="9">
+        <v>7</v>
+      </c>
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
       <c r="O41" s="12"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>11</v>
       </c>
@@ -1388,13 +1461,11 @@
       <c r="N42" s="9"/>
       <c r="O42" s="12"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>3</v>
       </c>
-      <c r="B43" s="9">
-        <v>3</v>
-      </c>
+      <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -1403,14 +1474,16 @@
       <c r="I43" s="6">
         <v>3</v>
       </c>
-      <c r="J43" s="9"/>
+      <c r="J43" s="9">
+        <v>14</v>
+      </c>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
       <c r="O43" s="12"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>14</v>
       </c>
@@ -1430,15 +1503,13 @@
       <c r="N44" s="9"/>
       <c r="O44" s="12"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>7</v>
       </c>
-      <c r="B45" s="9">
-        <v>10</v>
-      </c>
+      <c r="B45" s="9"/>
       <c r="C45" s="9">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -1447,14 +1518,18 @@
       <c r="I45" s="6">
         <v>7</v>
       </c>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
+      <c r="J45" s="9">
+        <v>7</v>
+      </c>
+      <c r="K45" s="9">
+        <v>7</v>
+      </c>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
       <c r="O45" s="12"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>10</v>
       </c>
@@ -1474,7 +1549,7 @@
       <c r="N46" s="9"/>
       <c r="O46" s="12"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>2</v>
       </c>
@@ -1489,14 +1564,16 @@
       <c r="I47" s="6">
         <v>2</v>
       </c>
-      <c r="J47" s="9"/>
+      <c r="J47" s="9">
+        <v>2</v>
+      </c>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
       <c r="O47" s="12"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>15</v>
       </c>
@@ -1516,7 +1593,7 @@
       <c r="N48" s="9"/>
       <c r="O48" s="12"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>1</v>
       </c>
@@ -1537,14 +1614,22 @@
       <c r="I49" s="8">
         <v>1</v>
       </c>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
+      <c r="J49" s="10">
+        <v>1</v>
+      </c>
+      <c r="K49" s="10">
+        <v>1</v>
+      </c>
+      <c r="L49" s="10">
+        <v>1</v>
+      </c>
+      <c r="M49" s="10">
+        <v>1</v>
+      </c>
       <c r="N49" s="9"/>
       <c r="O49" s="12"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>16</v>
       </c>
@@ -1564,13 +1649,11 @@
       <c r="N50" s="9"/>
       <c r="O50" s="12"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>8</v>
       </c>
-      <c r="B51" s="9">
-        <v>9</v>
-      </c>
+      <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
@@ -1579,14 +1662,16 @@
       <c r="I51" s="6">
         <v>8</v>
       </c>
-      <c r="J51" s="9"/>
+      <c r="J51" s="9">
+        <v>9</v>
+      </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
       <c r="O51" s="12"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>9</v>
       </c>
@@ -1606,7 +1691,7 @@
       <c r="N52" s="9"/>
       <c r="O52" s="12"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>5</v>
       </c>
@@ -1623,14 +1708,18 @@
       <c r="I53" s="6">
         <v>5</v>
       </c>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
+      <c r="J53" s="9">
+        <v>5</v>
+      </c>
+      <c r="K53" s="9">
+        <v>4</v>
+      </c>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
       <c r="O53" s="12"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>12</v>
       </c>
@@ -1650,13 +1739,11 @@
       <c r="N54" s="9"/>
       <c r="O54" s="12"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>4</v>
       </c>
-      <c r="B55" s="9">
-        <v>4</v>
-      </c>
+      <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
@@ -1665,14 +1752,16 @@
       <c r="I55" s="6">
         <v>4</v>
       </c>
-      <c r="J55" s="9"/>
+      <c r="J55" s="9">
+        <v>4</v>
+      </c>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
       <c r="O55" s="12"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>13</v>
       </c>
@@ -1692,18 +1781,14 @@
       <c r="N56" s="9"/>
       <c r="O56" s="12"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>6</v>
       </c>
-      <c r="B57" s="9">
-        <v>6</v>
-      </c>
-      <c r="C57" s="9">
-        <v>6</v>
-      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
       <c r="D57" s="9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
@@ -1711,14 +1796,20 @@
       <c r="I57" s="6">
         <v>6</v>
       </c>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
+      <c r="J57" s="9">
+        <v>6</v>
+      </c>
+      <c r="K57" s="9">
+        <v>6</v>
+      </c>
+      <c r="L57" s="9">
+        <v>2</v>
+      </c>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
       <c r="O57" s="12"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>11</v>
       </c>
@@ -1738,13 +1829,11 @@
       <c r="N58" s="9"/>
       <c r="O58" s="12"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>3</v>
       </c>
-      <c r="B59" s="9">
-        <v>3</v>
-      </c>
+      <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
@@ -1753,14 +1842,16 @@
       <c r="I59" s="6">
         <v>3</v>
       </c>
-      <c r="J59" s="9"/>
+      <c r="J59" s="9">
+        <v>3</v>
+      </c>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
       <c r="O59" s="12"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>14</v>
       </c>
@@ -1780,15 +1871,13 @@
       <c r="N60" s="9"/>
       <c r="O60" s="12"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>7</v>
       </c>
-      <c r="B61" s="9">
-        <v>7</v>
-      </c>
+      <c r="B61" s="9"/>
       <c r="C61" s="9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
@@ -1797,14 +1886,18 @@
       <c r="I61" s="6">
         <v>7</v>
       </c>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
+      <c r="J61" s="9">
+        <v>7</v>
+      </c>
+      <c r="K61" s="9">
+        <v>2</v>
+      </c>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
       <c r="O61" s="12"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>10</v>
       </c>
@@ -1824,7 +1917,7 @@
       <c r="N62" s="9"/>
       <c r="O62" s="12"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>2</v>
       </c>
@@ -1839,14 +1932,16 @@
       <c r="I63" s="6">
         <v>2</v>
       </c>
-      <c r="J63" s="9"/>
+      <c r="J63" s="9">
+        <v>2</v>
+      </c>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
       <c r="O63" s="12"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>15</v>
       </c>

</xml_diff>